<commit_message>
added functionality to 'Browse Files' button, implemented the conversion and download process
</commit_message>
<xml_diff>
--- a/src/xlsx/Template.xlsx
+++ b/src/xlsx/Template.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\GitHub\xlsx-to-qti\src\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8E2263-3114-4DB3-9318-EA745BC76234}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C62E5DB8-F0F5-4927-8CC6-C68E9D28D018}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3840" yWindow="3840" windowWidth="21600" windowHeight="11205" xr2:uid="{5C045D07-051C-4BB9-ABA4-3C26051C391C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{5C045D07-051C-4BB9-ABA4-3C26051C391C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Quiz Template" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="13">
   <si>
     <t>Question</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Explanation</t>
   </si>
   <si>
-    <t>Incorrect answer</t>
-  </si>
-  <si>
     <t>MCQ</t>
   </si>
   <si>
@@ -67,6 +64,15 @@
   </si>
   <si>
     <t>NOTE: Remember to rename this .xlsx file as the title of the quiz.</t>
+  </si>
+  <si>
+    <t>Incorrect answer 1</t>
+  </si>
+  <si>
+    <t>Incorrect answer 2</t>
+  </si>
+  <si>
+    <t>Incorrect answer 3</t>
   </si>
 </sst>
 </file>
@@ -471,13 +477,13 @@
     <col min="5" max="5" width="29.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="10" width="19.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" s="4"/>
       <c r="C1" s="4"/>
@@ -492,10 +498,10 @@
     </row>
     <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>0</v>
@@ -513,13 +519,13 @@
         <v>4</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="K2" s="3" t="s">
         <v>5</v>
@@ -527,7 +533,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -542,7 +548,7 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -557,7 +563,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -572,7 +578,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -587,7 +593,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -602,7 +608,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -617,7 +623,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -632,7 +638,7 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -647,7 +653,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -662,7 +668,7 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -677,7 +683,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -692,7 +698,7 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -707,7 +713,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -722,7 +728,7 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -737,7 +743,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -752,7 +758,7 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -767,7 +773,7 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -782,7 +788,7 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -797,7 +803,7 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -812,7 +818,7 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -827,7 +833,7 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -842,7 +848,7 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -857,7 +863,7 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -872,7 +878,7 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -887,7 +893,7 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -902,7 +908,7 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -917,7 +923,7 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -932,7 +938,7 @@
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -947,7 +953,7 @@
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -962,7 +968,7 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -977,7 +983,7 @@
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -992,7 +998,7 @@
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -1007,7 +1013,7 @@
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1022,7 +1028,7 @@
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -1037,7 +1043,7 @@
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -1052,7 +1058,7 @@
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -1067,7 +1073,7 @@
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -1082,7 +1088,7 @@
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
@@ -1097,7 +1103,7 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
@@ -1112,7 +1118,7 @@
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B42" s="1"/>
       <c r="C42" s="1"/>
@@ -1127,7 +1133,7 @@
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -1142,7 +1148,7 @@
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -1157,7 +1163,7 @@
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -1172,7 +1178,7 @@
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -1187,7 +1193,7 @@
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -1202,7 +1208,7 @@
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B48" s="1"/>
       <c r="C48" s="1"/>
@@ -1217,7 +1223,7 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -1232,7 +1238,7 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -1247,7 +1253,7 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1262,7 +1268,7 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="1"/>
@@ -1277,7 +1283,7 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B53" s="1"/>
       <c r="C53" s="1"/>
@@ -1292,7 +1298,7 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B54" s="1"/>
       <c r="C54" s="1"/>
@@ -1307,7 +1313,7 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B55" s="1"/>
       <c r="C55" s="1"/>
@@ -1322,7 +1328,7 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B56" s="1"/>
       <c r="C56" s="1"/>
@@ -1337,7 +1343,7 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -1352,7 +1358,7 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -1367,7 +1373,7 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -1382,7 +1388,7 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -1397,7 +1403,7 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -1412,7 +1418,7 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -1427,7 +1433,7 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -1442,7 +1448,7 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -1457,7 +1463,7 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -1472,7 +1478,7 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -1487,7 +1493,7 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -1502,7 +1508,7 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -1517,7 +1523,7 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -1532,7 +1538,7 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -1547,7 +1553,7 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -1562,7 +1568,7 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B72" s="1"/>
       <c r="C72" s="1"/>
@@ -1577,7 +1583,7 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
@@ -1592,7 +1598,7 @@
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B74" s="1"/>
       <c r="C74" s="1"/>
@@ -1607,7 +1613,7 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B75" s="1"/>
       <c r="C75" s="1"/>
@@ -1622,7 +1628,7 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B76" s="1"/>
       <c r="C76" s="1"/>
@@ -1637,7 +1643,7 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B77" s="1"/>
       <c r="C77" s="1"/>
@@ -1652,7 +1658,7 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
@@ -1667,7 +1673,7 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B79" s="1"/>
       <c r="C79" s="1"/>
@@ -1682,7 +1688,7 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -1697,7 +1703,7 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -1712,7 +1718,7 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B82" s="1"/>
       <c r="C82" s="1"/>
@@ -1727,7 +1733,7 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B83" s="1"/>
       <c r="C83" s="1"/>
@@ -1742,7 +1748,7 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B84" s="1"/>
       <c r="C84" s="1"/>
@@ -1757,7 +1763,7 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B85" s="1"/>
       <c r="C85" s="1"/>
@@ -1772,7 +1778,7 @@
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B86" s="1"/>
       <c r="C86" s="1"/>
@@ -1787,7 +1793,7 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B87" s="1"/>
       <c r="C87" s="1"/>
@@ -1802,7 +1808,7 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B88" s="1"/>
       <c r="C88" s="1"/>
@@ -1817,7 +1823,7 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B89" s="1"/>
       <c r="C89" s="1"/>
@@ -1832,7 +1838,7 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B90" s="1"/>
       <c r="C90" s="1"/>
@@ -1847,7 +1853,7 @@
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B91" s="1"/>
       <c r="C91" s="1"/>
@@ -1862,7 +1868,7 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B92" s="1"/>
       <c r="C92" s="1"/>
@@ -1877,7 +1883,7 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B93" s="1"/>
       <c r="C93" s="1"/>
@@ -1892,7 +1898,7 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B94" s="1"/>
       <c r="C94" s="1"/>
@@ -1907,7 +1913,7 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B95" s="1"/>
       <c r="C95" s="1"/>
@@ -1922,7 +1928,7 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B96" s="1"/>
       <c r="C96" s="1"/>
@@ -1937,7 +1943,7 @@
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B97" s="1"/>
       <c r="C97" s="1"/>
@@ -1952,7 +1958,7 @@
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B98" s="1"/>
       <c r="C98" s="1"/>
@@ -1967,7 +1973,7 @@
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B99" s="1"/>
       <c r="C99" s="1"/>
@@ -1982,7 +1988,7 @@
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B100" s="1"/>
       <c r="C100" s="1"/>
@@ -1997,7 +2003,7 @@
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -2012,7 +2018,7 @@
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B102" s="1"/>
       <c r="C102" s="1"/>
@@ -2027,7 +2033,7 @@
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B103" s="1"/>
       <c r="C103" s="1"/>
@@ -2042,7 +2048,7 @@
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B104" s="1"/>
       <c r="C104" s="1"/>
@@ -2057,7 +2063,7 @@
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B105" s="1"/>
       <c r="C105" s="1"/>
@@ -2072,7 +2078,7 @@
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B106" s="1"/>
       <c r="C106" s="1"/>
@@ -2087,7 +2093,7 @@
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B107" s="1"/>
       <c r="C107" s="1"/>
@@ -2102,7 +2108,7 @@
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B108" s="1"/>
       <c r="C108" s="1"/>
@@ -2117,7 +2123,7 @@
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B109" s="1"/>
       <c r="C109" s="1"/>
@@ -2132,7 +2138,7 @@
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B110" s="1"/>
       <c r="C110" s="1"/>
@@ -2147,7 +2153,7 @@
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B111" s="1"/>
       <c r="C111" s="1"/>
@@ -2162,7 +2168,7 @@
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B112" s="1"/>
       <c r="C112" s="1"/>
@@ -2177,7 +2183,7 @@
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B113" s="1"/>
       <c r="C113" s="1"/>
@@ -2192,7 +2198,7 @@
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B114" s="1"/>
       <c r="C114" s="1"/>
@@ -2207,7 +2213,7 @@
     </row>
     <row r="115" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B115" s="1"/>
       <c r="C115" s="1"/>
@@ -2222,7 +2228,7 @@
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B116" s="1"/>
       <c r="C116" s="1"/>
@@ -2237,7 +2243,7 @@
     </row>
     <row r="117" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B117" s="1"/>
       <c r="C117" s="1"/>
@@ -2252,7 +2258,7 @@
     </row>
     <row r="118" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B118" s="1"/>
       <c r="C118" s="1"/>
@@ -2267,7 +2273,7 @@
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B119" s="1"/>
       <c r="C119" s="1"/>
@@ -2282,7 +2288,7 @@
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B120" s="1"/>
       <c r="C120" s="1"/>
@@ -2297,7 +2303,7 @@
     </row>
     <row r="121" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B121" s="1"/>
       <c r="C121" s="1"/>
@@ -2312,7 +2318,7 @@
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B122" s="1"/>
       <c r="C122" s="1"/>
@@ -2327,7 +2333,7 @@
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B123" s="1"/>
       <c r="C123" s="1"/>
@@ -2342,7 +2348,7 @@
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B124" s="1"/>
       <c r="C124" s="1"/>
@@ -2357,7 +2363,7 @@
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B125" s="1"/>
       <c r="C125" s="1"/>
@@ -2372,7 +2378,7 @@
     </row>
     <row r="126" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
@@ -2387,7 +2393,7 @@
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
@@ -2402,7 +2408,7 @@
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B128" s="1"/>
       <c r="C128" s="1"/>
@@ -2417,7 +2423,7 @@
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B129" s="1"/>
       <c r="C129" s="1"/>
@@ -2432,7 +2438,7 @@
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B130" s="1"/>
       <c r="C130" s="1"/>
@@ -2447,7 +2453,7 @@
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B131" s="1"/>
       <c r="C131" s="1"/>
@@ -2462,7 +2468,7 @@
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B132" s="1"/>
       <c r="C132" s="1"/>
@@ -2477,7 +2483,7 @@
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B133" s="1"/>
       <c r="C133" s="1"/>
@@ -2492,7 +2498,7 @@
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B134" s="1"/>
       <c r="C134" s="1"/>
@@ -2507,7 +2513,7 @@
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B135" s="1"/>
       <c r="C135" s="1"/>
@@ -2522,7 +2528,7 @@
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B136" s="1"/>
       <c r="C136" s="1"/>
@@ -2537,7 +2543,7 @@
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B137" s="1"/>
       <c r="C137" s="1"/>
@@ -2552,7 +2558,7 @@
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B138" s="1"/>
       <c r="C138" s="1"/>
@@ -2567,7 +2573,7 @@
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B139" s="1"/>
       <c r="C139" s="1"/>
@@ -2582,7 +2588,7 @@
     </row>
     <row r="140" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B140" s="1"/>
       <c r="C140" s="1"/>
@@ -2597,7 +2603,7 @@
     </row>
     <row r="141" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B141" s="1"/>
       <c r="C141" s="1"/>
@@ -2612,7 +2618,7 @@
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B142" s="1"/>
       <c r="C142" s="1"/>
@@ -2627,7 +2633,7 @@
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B143" s="1"/>
       <c r="C143" s="1"/>
@@ -2642,7 +2648,7 @@
     </row>
     <row r="144" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B144" s="1"/>
       <c r="C144" s="1"/>
@@ -2657,7 +2663,7 @@
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B145" s="1"/>
       <c r="C145" s="1"/>
@@ -2672,7 +2678,7 @@
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B146" s="1"/>
       <c r="C146" s="1"/>
@@ -2687,7 +2693,7 @@
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B147" s="1"/>
       <c r="C147" s="1"/>
@@ -2702,7 +2708,7 @@
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B148" s="1"/>
       <c r="C148" s="1"/>
@@ -2717,7 +2723,7 @@
     </row>
     <row r="149" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B149" s="1"/>
       <c r="C149" s="1"/>
@@ -2732,7 +2738,7 @@
     </row>
     <row r="150" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B150" s="1"/>
       <c r="C150" s="1"/>
@@ -2747,7 +2753,7 @@
     </row>
     <row r="151" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B151" s="1"/>
       <c r="C151" s="1"/>
@@ -2762,7 +2768,7 @@
     </row>
     <row r="152" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B152" s="1"/>
       <c r="C152" s="1"/>
@@ -2777,7 +2783,7 @@
     </row>
     <row r="153" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B153" s="1"/>
       <c r="C153" s="1"/>
@@ -2792,7 +2798,7 @@
     </row>
     <row r="154" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B154" s="1"/>
       <c r="C154" s="1"/>
@@ -2807,7 +2813,7 @@
     </row>
     <row r="155" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B155" s="1"/>
       <c r="C155" s="1"/>
@@ -2822,7 +2828,7 @@
     </row>
     <row r="156" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B156" s="1"/>
       <c r="C156" s="1"/>
@@ -2837,7 +2843,7 @@
     </row>
     <row r="157" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B157" s="1"/>
       <c r="C157" s="1"/>
@@ -2852,7 +2858,7 @@
     </row>
     <row r="158" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B158" s="1"/>
       <c r="C158" s="1"/>
@@ -2867,7 +2873,7 @@
     </row>
     <row r="159" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B159" s="1"/>
       <c r="C159" s="1"/>
@@ -2882,7 +2888,7 @@
     </row>
     <row r="160" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B160" s="1"/>
       <c r="C160" s="1"/>
@@ -2897,7 +2903,7 @@
     </row>
     <row r="161" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B161" s="1"/>
       <c r="C161" s="1"/>
@@ -2912,7 +2918,7 @@
     </row>
     <row r="162" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B162" s="1"/>
       <c r="C162" s="1"/>
@@ -2927,7 +2933,7 @@
     </row>
     <row r="163" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B163" s="1"/>
       <c r="C163" s="1"/>
@@ -2942,7 +2948,7 @@
     </row>
     <row r="164" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B164" s="1"/>
       <c r="C164" s="1"/>
@@ -2957,7 +2963,7 @@
     </row>
     <row r="165" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B165" s="1"/>
       <c r="C165" s="1"/>
@@ -2972,7 +2978,7 @@
     </row>
     <row r="166" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B166" s="1"/>
       <c r="C166" s="1"/>
@@ -2987,7 +2993,7 @@
     </row>
     <row r="167" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B167" s="1"/>
       <c r="C167" s="1"/>
@@ -3002,7 +3008,7 @@
     </row>
     <row r="168" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B168" s="1"/>
       <c r="C168" s="1"/>
@@ -3017,7 +3023,7 @@
     </row>
     <row r="169" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B169" s="1"/>
       <c r="C169" s="1"/>
@@ -3032,7 +3038,7 @@
     </row>
     <row r="170" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B170" s="1"/>
       <c r="C170" s="1"/>
@@ -3047,7 +3053,7 @@
     </row>
     <row r="171" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B171" s="1"/>
       <c r="C171" s="1"/>
@@ -3062,7 +3068,7 @@
     </row>
     <row r="172" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B172" s="1"/>
       <c r="C172" s="1"/>
@@ -3077,7 +3083,7 @@
     </row>
     <row r="173" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B173" s="1"/>
       <c r="C173" s="1"/>
@@ -3092,7 +3098,7 @@
     </row>
     <row r="174" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B174" s="1"/>
       <c r="C174" s="1"/>
@@ -3107,7 +3113,7 @@
     </row>
     <row r="175" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B175" s="1"/>
       <c r="C175" s="1"/>
@@ -3122,7 +3128,7 @@
     </row>
     <row r="176" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B176" s="1"/>
       <c r="C176" s="1"/>
@@ -3137,7 +3143,7 @@
     </row>
     <row r="177" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B177" s="1"/>
       <c r="C177" s="1"/>
@@ -3152,7 +3158,7 @@
     </row>
     <row r="178" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B178" s="1"/>
       <c r="C178" s="1"/>
@@ -3167,7 +3173,7 @@
     </row>
     <row r="179" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B179" s="1"/>
       <c r="C179" s="1"/>
@@ -3182,7 +3188,7 @@
     </row>
     <row r="180" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B180" s="1"/>
       <c r="C180" s="1"/>
@@ -3197,7 +3203,7 @@
     </row>
     <row r="181" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B181" s="1"/>
       <c r="C181" s="1"/>
@@ -3212,7 +3218,7 @@
     </row>
     <row r="182" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B182" s="1"/>
       <c r="C182" s="1"/>
@@ -3227,7 +3233,7 @@
     </row>
     <row r="183" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B183" s="1"/>
       <c r="C183" s="1"/>
@@ -3242,7 +3248,7 @@
     </row>
     <row r="184" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B184" s="1"/>
       <c r="C184" s="1"/>
@@ -3257,7 +3263,7 @@
     </row>
     <row r="185" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B185" s="1"/>
       <c r="C185" s="1"/>
@@ -3272,7 +3278,7 @@
     </row>
     <row r="186" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B186" s="1"/>
       <c r="C186" s="1"/>
@@ -3287,7 +3293,7 @@
     </row>
     <row r="187" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B187" s="1"/>
       <c r="C187" s="1"/>
@@ -3302,7 +3308,7 @@
     </row>
     <row r="188" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B188" s="1"/>
       <c r="C188" s="1"/>
@@ -3317,7 +3323,7 @@
     </row>
     <row r="189" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B189" s="1"/>
       <c r="C189" s="1"/>
@@ -3332,7 +3338,7 @@
     </row>
     <row r="190" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B190" s="1"/>
       <c r="C190" s="1"/>
@@ -3347,7 +3353,7 @@
     </row>
     <row r="191" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B191" s="1"/>
       <c r="C191" s="1"/>
@@ -3362,7 +3368,7 @@
     </row>
     <row r="192" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A192" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B192" s="1"/>
       <c r="C192" s="1"/>
@@ -3377,7 +3383,7 @@
     </row>
     <row r="193" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A193" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B193" s="1"/>
       <c r="C193" s="1"/>
@@ -3392,7 +3398,7 @@
     </row>
     <row r="194" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A194" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B194" s="1"/>
       <c r="C194" s="1"/>
@@ -3407,7 +3413,7 @@
     </row>
     <row r="195" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A195" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B195" s="1"/>
       <c r="C195" s="1"/>
@@ -3422,7 +3428,7 @@
     </row>
     <row r="196" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A196" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B196" s="1"/>
       <c r="C196" s="1"/>
@@ -3437,7 +3443,7 @@
     </row>
     <row r="197" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A197" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B197" s="1"/>
       <c r="C197" s="1"/>
@@ -3452,7 +3458,7 @@
     </row>
     <row r="198" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A198" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B198" s="1"/>
       <c r="C198" s="1"/>
@@ -3467,7 +3473,7 @@
     </row>
     <row r="199" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A199" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B199" s="1"/>
       <c r="C199" s="1"/>
@@ -3482,7 +3488,7 @@
     </row>
     <row r="200" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A200" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B200" s="1"/>
       <c r="C200" s="1"/>
@@ -3497,7 +3503,7 @@
     </row>
     <row r="201" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A201" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B201" s="1"/>
       <c r="C201" s="1"/>
@@ -3512,7 +3518,7 @@
     </row>
     <row r="202" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A202" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B202" s="1"/>
       <c r="C202" s="1"/>
@@ -3527,7 +3533,7 @@
     </row>
     <row r="203" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A203" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B203" s="1"/>
       <c r="C203" s="1"/>
@@ -3542,7 +3548,7 @@
     </row>
     <row r="204" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A204" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B204" s="1"/>
       <c r="C204" s="1"/>
@@ -3557,7 +3563,7 @@
     </row>
     <row r="205" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A205" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B205" s="1"/>
       <c r="C205" s="1"/>
@@ -3572,7 +3578,7 @@
     </row>
     <row r="206" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A206" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B206" s="1"/>
       <c r="C206" s="1"/>
@@ -3587,7 +3593,7 @@
     </row>
     <row r="207" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A207" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B207" s="1"/>
       <c r="C207" s="1"/>
@@ -3602,7 +3608,7 @@
     </row>
     <row r="208" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A208" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B208" s="1"/>
       <c r="C208" s="1"/>
@@ -3617,7 +3623,7 @@
     </row>
     <row r="209" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A209" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B209" s="1"/>
       <c r="C209" s="1"/>
@@ -3632,7 +3638,7 @@
     </row>
     <row r="210" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A210" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B210" s="1"/>
       <c r="C210" s="1"/>
@@ -3647,7 +3653,7 @@
     </row>
     <row r="211" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A211" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B211" s="1"/>
       <c r="C211" s="1"/>
@@ -3662,7 +3668,7 @@
     </row>
     <row r="212" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A212" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B212" s="1"/>
       <c r="C212" s="1"/>
@@ -3677,7 +3683,7 @@
     </row>
     <row r="213" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A213" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B213" s="1"/>
       <c r="C213" s="1"/>
@@ -3692,7 +3698,7 @@
     </row>
     <row r="214" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A214" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B214" s="1"/>
       <c r="C214" s="1"/>
@@ -3707,7 +3713,7 @@
     </row>
     <row r="215" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A215" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B215" s="1"/>
       <c r="C215" s="1"/>
@@ -3722,7 +3728,7 @@
     </row>
     <row r="216" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A216" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B216" s="1"/>
       <c r="C216" s="1"/>
@@ -3737,7 +3743,7 @@
     </row>
     <row r="217" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A217" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B217" s="1"/>
       <c r="C217" s="1"/>
@@ -3752,7 +3758,7 @@
     </row>
     <row r="218" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A218" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B218" s="1"/>
       <c r="C218" s="1"/>
@@ -3767,7 +3773,7 @@
     </row>
     <row r="219" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A219" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B219" s="1"/>
       <c r="C219" s="1"/>
@@ -3782,7 +3788,7 @@
     </row>
     <row r="220" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A220" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B220" s="1"/>
       <c r="C220" s="1"/>
@@ -3797,7 +3803,7 @@
     </row>
     <row r="221" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A221" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B221" s="1"/>
       <c r="C221" s="1"/>
@@ -3812,7 +3818,7 @@
     </row>
     <row r="222" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A222" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B222" s="1"/>
       <c r="C222" s="1"/>
@@ -3827,7 +3833,7 @@
     </row>
     <row r="223" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A223" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B223" s="1"/>
       <c r="C223" s="1"/>
@@ -3842,7 +3848,7 @@
     </row>
     <row r="224" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A224" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B224" s="1"/>
       <c r="C224" s="1"/>
@@ -3857,7 +3863,7 @@
     </row>
     <row r="225" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A225" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B225" s="1"/>
       <c r="C225" s="1"/>
@@ -3872,7 +3878,7 @@
     </row>
     <row r="226" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A226" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B226" s="1"/>
       <c r="C226" s="1"/>
@@ -3887,7 +3893,7 @@
     </row>
     <row r="227" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A227" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B227" s="1"/>
       <c r="C227" s="1"/>
@@ -3902,7 +3908,7 @@
     </row>
     <row r="228" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A228" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B228" s="1"/>
       <c r="C228" s="1"/>
@@ -3917,7 +3923,7 @@
     </row>
     <row r="229" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A229" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B229" s="1"/>
       <c r="C229" s="1"/>
@@ -3932,7 +3938,7 @@
     </row>
     <row r="230" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A230" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B230" s="1"/>
       <c r="C230" s="1"/>
@@ -3947,7 +3953,7 @@
     </row>
     <row r="231" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A231" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B231" s="1"/>
       <c r="C231" s="1"/>
@@ -3962,7 +3968,7 @@
     </row>
     <row r="232" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A232" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B232" s="1"/>
       <c r="C232" s="1"/>
@@ -3977,7 +3983,7 @@
     </row>
     <row r="233" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A233" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B233" s="1"/>
       <c r="C233" s="1"/>
@@ -3992,7 +3998,7 @@
     </row>
     <row r="234" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A234" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B234" s="1"/>
       <c r="C234" s="1"/>
@@ -4007,7 +4013,7 @@
     </row>
     <row r="235" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A235" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B235" s="1"/>
       <c r="C235" s="1"/>
@@ -4022,7 +4028,7 @@
     </row>
     <row r="236" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A236" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B236" s="1"/>
       <c r="C236" s="1"/>
@@ -4037,7 +4043,7 @@
     </row>
     <row r="237" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A237" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B237" s="1"/>
       <c r="C237" s="1"/>
@@ -4052,7 +4058,7 @@
     </row>
     <row r="238" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A238" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B238" s="1"/>
       <c r="C238" s="1"/>
@@ -4067,7 +4073,7 @@
     </row>
     <row r="239" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A239" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B239" s="1"/>
       <c r="C239" s="1"/>
@@ -4082,7 +4088,7 @@
     </row>
     <row r="240" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A240" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B240" s="1"/>
       <c r="C240" s="1"/>
@@ -4097,7 +4103,7 @@
     </row>
     <row r="241" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A241" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B241" s="1"/>
       <c r="C241" s="1"/>
@@ -4112,7 +4118,7 @@
     </row>
     <row r="242" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A242" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B242" s="1"/>
       <c r="C242" s="1"/>
@@ -4127,7 +4133,7 @@
     </row>
     <row r="243" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A243" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B243" s="1"/>
       <c r="C243" s="1"/>
@@ -4142,7 +4148,7 @@
     </row>
     <row r="244" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A244" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B244" s="1"/>
       <c r="C244" s="1"/>
@@ -4157,7 +4163,7 @@
     </row>
     <row r="245" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A245" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B245" s="1"/>
       <c r="C245" s="1"/>
@@ -4172,7 +4178,7 @@
     </row>
     <row r="246" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A246" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B246" s="1"/>
       <c r="C246" s="1"/>
@@ -4187,7 +4193,7 @@
     </row>
     <row r="247" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A247" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B247" s="1"/>
       <c r="C247" s="1"/>
@@ -4202,7 +4208,7 @@
     </row>
     <row r="248" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A248" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B248" s="1"/>
       <c r="C248" s="1"/>

</xml_diff>